<commit_message>
Version 3.2. Adds prey size adjustment feature to account for known size biases
</commit_message>
<xml_diff>
--- a/helperfiles/Adjust_size_prey.xlsx
+++ b/helperfiles/Adjust_size_prey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhydra-my.sharepoint.com/personal/ttinker_nhydra-eco_com/Documents/SOFA2/SOFA/helperfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{D04806A4-ADE5-4176-8557-F3340D44A6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{949B4FB7-9C85-4F9B-A4B5-937DC1797F61}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{E5781423-6B54-43FD-8DCC-BC21D3736D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F3CABE6-8B13-4991-B7E4-7B8739525A55}"/>
   <bookViews>
     <workbookView xWindow="5610" yWindow="2790" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>Tim Tinker</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A9D9D83F-75F8-41AD-86FB-363069F0B42C}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{10100DEA-DFD1-4D75-9030-65844139F3D2}">
       <text>
         <r>
           <rPr>
@@ -59,11 +59,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-enter the prey type code for prey to be size-adjusted at the specified group level</t>
+Enter the grouping variable used to select prey for size-adjustment (leave blank for global adjustment)... examples include Region, Area, Period, Site, Ottername... </t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E94FDA47-477E-440C-98A6-60962C853C88}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{0D0C1627-7DD9-4C81-96BE-675FDAE65553}">
       <text>
         <r>
           <rPr>
@@ -83,7 +83,55 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Enter the factor to multiply prey diameter by (1.1 = multiply prey diameter by 1.1, to make it 10% bigger)</t>
+Enter the value of the grouping variable used to select prey (leave blank for global adjustment)…</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A9D9D83F-75F8-41AD-86FB-363069F0B42C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tim Tinker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+enter the prey type code for prey to be size-adjusted (either globally or at the specified group level). Must match one of the prey type codes from Prey_Key</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{E94FDA47-477E-440C-98A6-60962C853C88}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tim Tinker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enter the factor to multiply prey diameter by (e.g. enter 1.1 to multiply prey diameter by 1.1, to make it 10% bigger)</t>
         </r>
       </text>
     </comment>
@@ -92,7 +140,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Groupvar</t>
+  </si>
   <si>
     <t>PreyType</t>
   </si>
@@ -100,7 +151,7 @@
     <t>Adjust_fact</t>
   </si>
   <si>
-    <t>sna</t>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -431,32 +482,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>